<commit_message>
updated grade and hw3
</commit_message>
<xml_diff>
--- a/grade.xlsx
+++ b/grade.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/twhuang/PhD/Course/ECE5960/spring20/ece5960/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7609EA83-9AA5-7549-997D-4C6C6F8DCED8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B1A3BDD-A52A-2345-BA23-B522E49FE9ED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="13880" yWindow="3780" windowWidth="25600" windowHeight="15540" xr2:uid="{20F95EEC-55CF-F545-8D24-5394123A7EB4}"/>
   </bookViews>
@@ -426,7 +426,7 @@
   <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -714,6 +714,9 @@
       <c r="L9">
         <v>100</v>
       </c>
+      <c r="M9">
+        <v>100</v>
+      </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10">
@@ -791,6 +794,9 @@
         <v>100</v>
       </c>
       <c r="L11">
+        <v>100</v>
+      </c>
+      <c r="M11">
         <v>100</v>
       </c>
     </row>

</xml_diff>